<commit_message>
Intro to ML completed
</commit_message>
<xml_diff>
--- a/projects/Project3_visualizing-real-world-data-project/Data/HK House Prices Clean.xlsx
+++ b/projects/Project3_visualizing-real-world-data-project/Data/HK House Prices Clean.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borelliandrea/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borelliandrea/Ironhack/dataptams2020/projects/Project3_visualizing-real-world-data-project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA397305-2D44-BC43-993E-50CBAF83F34C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BE8C34-75F3-F74E-BB2B-8B66B817683E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0CCF993D-5DC6-824F-BC17-EEDFBBD7F891}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{0CCF993D-5DC6-824F-BC17-EEDFBBD7F891}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Quarter</t>
@@ -88,6 +85,9 @@
   <si>
     <t>&lt;40_New_Territories</t>
   </si>
+  <si>
+    <t>Average Sales House Prices</t>
+  </si>
 </sst>
 </file>
 
@@ -129,10 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,62 +451,68 @@
   <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A29"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -560,6 +567,9 @@
       <c r="Q2">
         <v>47795</v>
       </c>
+      <c r="R2" s="3">
+        <v>49244.866666666669</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -613,6 +623,9 @@
       <c r="Q3">
         <v>47953</v>
       </c>
+      <c r="R3" s="3">
+        <v>50842.2</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -666,6 +679,9 @@
       <c r="Q4">
         <v>46212</v>
       </c>
+      <c r="R4" s="3">
+        <v>48925.4</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -719,6 +735,9 @@
       <c r="Q5">
         <v>47712</v>
       </c>
+      <c r="R5" s="3">
+        <v>48324.2</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -772,6 +791,9 @@
       <c r="Q6">
         <v>47982</v>
       </c>
+      <c r="R6" s="3">
+        <v>48305.066666666666</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -825,6 +847,9 @@
       <c r="Q7">
         <v>46880</v>
       </c>
+      <c r="R7" s="3">
+        <v>45287.666666666664</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -878,8 +903,8 @@
       <c r="Q8">
         <v>43305</v>
       </c>
-      <c r="R8" t="s">
-        <v>1</v>
+      <c r="R8" s="3">
+        <v>44462.6</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -934,8 +959,8 @@
       <c r="Q9">
         <v>40074</v>
       </c>
-      <c r="R9" t="s">
-        <v>1</v>
+      <c r="R9" s="3">
+        <v>44051.066666666666</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -990,6 +1015,9 @@
       <c r="Q10">
         <v>34009</v>
       </c>
+      <c r="R10" s="3">
+        <v>40274.400000000001</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1043,6 +1071,9 @@
       <c r="Q11">
         <v>35534</v>
       </c>
+      <c r="R11" s="3">
+        <v>40961.666666666664</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1096,6 +1127,9 @@
       <c r="Q12">
         <v>32621</v>
       </c>
+      <c r="R12" s="3">
+        <v>39317.533333333333</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1149,6 +1183,9 @@
       <c r="Q13">
         <v>39134</v>
       </c>
+      <c r="R13" s="3">
+        <v>37789.199999999997</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1202,8 +1239,8 @@
       <c r="Q14">
         <v>35754</v>
       </c>
-      <c r="R14" t="s">
-        <v>1</v>
+      <c r="R14" s="3">
+        <v>36610.533333333333</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -1258,8 +1295,8 @@
       <c r="Q15">
         <v>38117</v>
       </c>
-      <c r="R15" t="s">
-        <v>1</v>
+      <c r="R15" s="3">
+        <v>36755.933333333334</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -1314,8 +1351,8 @@
       <c r="Q16">
         <v>33530</v>
       </c>
-      <c r="R16" t="s">
-        <v>1</v>
+      <c r="R16" s="3">
+        <v>34530.73333333333</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -1370,8 +1407,8 @@
       <c r="Q17">
         <v>33041</v>
       </c>
-      <c r="R17" t="s">
-        <v>1</v>
+      <c r="R17" s="3">
+        <v>34447.4</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -1426,8 +1463,8 @@
       <c r="Q18">
         <v>34525</v>
       </c>
-      <c r="R18" t="s">
-        <v>1</v>
+      <c r="R18" s="3">
+        <v>33248.466666666667</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -1482,8 +1519,8 @@
       <c r="Q19">
         <v>29708</v>
       </c>
-      <c r="R19" t="s">
-        <v>1</v>
+      <c r="R19" s="3">
+        <v>30702.333333333332</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -1538,8 +1575,8 @@
       <c r="Q20">
         <v>32861</v>
       </c>
-      <c r="R20" t="s">
-        <v>1</v>
+      <c r="R20" s="3">
+        <v>32215.933333333334</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -1594,8 +1631,8 @@
       <c r="Q21">
         <v>37137</v>
       </c>
-      <c r="R21" t="s">
-        <v>1</v>
+      <c r="R21" s="3">
+        <v>36423.133333333331</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -1650,8 +1687,8 @@
       <c r="Q22">
         <v>42683</v>
       </c>
-      <c r="R22" t="s">
-        <v>1</v>
+      <c r="R22" s="3">
+        <v>43693.26666666667</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -1706,8 +1743,8 @@
       <c r="Q23">
         <v>37298</v>
       </c>
-      <c r="R23" t="s">
-        <v>1</v>
+      <c r="R23" s="3">
+        <v>44512.333333333336</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
@@ -1762,8 +1799,8 @@
       <c r="Q24">
         <v>46614</v>
       </c>
-      <c r="R24" t="s">
-        <v>1</v>
+      <c r="R24" s="3">
+        <v>46761.666666666664</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
@@ -1818,8 +1855,8 @@
       <c r="Q25">
         <v>48227</v>
       </c>
-      <c r="R25" t="s">
-        <v>1</v>
+      <c r="R25" s="3">
+        <v>53334.333333333336</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
@@ -1874,6 +1911,9 @@
       <c r="Q26">
         <v>50970</v>
       </c>
+      <c r="R26" s="3">
+        <v>54906.933333333334</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
@@ -1927,6 +1967,9 @@
       <c r="Q27">
         <v>63346</v>
       </c>
+      <c r="R27" s="3">
+        <v>58843</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
@@ -1980,6 +2023,9 @@
       <c r="Q28">
         <v>58356</v>
       </c>
+      <c r="R28" s="3">
+        <v>58958.666666666664</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
@@ -2033,6 +2079,9 @@
       <c r="Q29">
         <v>52487</v>
       </c>
+      <c r="R29" s="3">
+        <v>56269.933333333334</v>
+      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -2086,6 +2135,9 @@
       <c r="Q30">
         <v>52490</v>
       </c>
+      <c r="R30" s="3">
+        <v>57703.666666666664</v>
+      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -2139,6 +2191,9 @@
       <c r="Q31">
         <v>56682</v>
       </c>
+      <c r="R31" s="3">
+        <v>59179.866666666669</v>
+      </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -2192,6 +2247,9 @@
       <c r="Q32">
         <v>58420</v>
       </c>
+      <c r="R32" s="3">
+        <v>59347.199999999997</v>
+      </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -2245,6 +2303,9 @@
       <c r="Q33">
         <v>56143</v>
       </c>
+      <c r="R33" s="3">
+        <v>57748.466666666667</v>
+      </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -2298,8 +2359,8 @@
       <c r="Q34">
         <v>65108</v>
       </c>
-      <c r="R34" t="s">
-        <v>1</v>
+      <c r="R34" s="3">
+        <v>62141.533333333333</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
@@ -2354,8 +2415,8 @@
       <c r="Q35">
         <v>58146</v>
       </c>
-      <c r="R35" t="s">
-        <v>1</v>
+      <c r="R35" s="3">
+        <v>64873.666666666664</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
@@ -2410,8 +2471,8 @@
       <c r="Q36">
         <v>65876</v>
       </c>
-      <c r="R36" t="s">
-        <v>1</v>
+      <c r="R36" s="3">
+        <v>69742.066666666666</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
@@ -2466,8 +2527,8 @@
       <c r="Q37">
         <v>81762</v>
       </c>
-      <c r="R37" t="s">
-        <v>1</v>
+      <c r="R37" s="3">
+        <v>81718.866666666669</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -2522,8 +2583,8 @@
       <c r="Q38">
         <v>82989</v>
       </c>
-      <c r="R38" t="s">
-        <v>1</v>
+      <c r="R38" s="3">
+        <v>82858.600000000006</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
@@ -2578,8 +2639,8 @@
       <c r="Q39">
         <v>77095</v>
       </c>
-      <c r="R39" t="s">
-        <v>1</v>
+      <c r="R39" s="3">
+        <v>83829.600000000006</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
@@ -2634,8 +2695,8 @@
       <c r="Q40">
         <v>64094</v>
       </c>
-      <c r="R40" t="s">
-        <v>1</v>
+      <c r="R40" s="3">
+        <v>80666.2</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
@@ -2690,8 +2751,8 @@
       <c r="Q41">
         <v>54006</v>
       </c>
-      <c r="R41" t="s">
-        <v>1</v>
+      <c r="R41" s="3">
+        <v>68056.266666666663</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
@@ -2746,8 +2807,8 @@
       <c r="Q42">
         <v>61014</v>
       </c>
-      <c r="R42" t="s">
-        <v>1</v>
+      <c r="R42" s="3">
+        <v>69661.133333333331</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
@@ -2802,8 +2863,8 @@
       <c r="Q43">
         <v>69176</v>
       </c>
-      <c r="R43" t="s">
-        <v>1</v>
+      <c r="R43" s="3">
+        <v>77540.2</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -2858,6 +2919,9 @@
       <c r="Q44">
         <v>71671</v>
       </c>
+      <c r="R44" s="3">
+        <v>83516.133333333331</v>
+      </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45">
@@ -2911,6 +2975,9 @@
       <c r="Q45">
         <v>70567</v>
       </c>
+      <c r="R45" s="3">
+        <v>86602.066666666666</v>
+      </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46">
@@ -2964,6 +3031,9 @@
       <c r="Q46">
         <v>78727</v>
       </c>
+      <c r="R46" s="3">
+        <v>93077.6</v>
+      </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47">
@@ -3017,8 +3087,8 @@
       <c r="Q47">
         <v>66992</v>
       </c>
-      <c r="R47" t="s">
-        <v>1</v>
+      <c r="R47" s="3">
+        <v>92334.8</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
@@ -3073,8 +3143,8 @@
       <c r="Q48">
         <v>74008</v>
       </c>
-      <c r="R48" t="s">
-        <v>1</v>
+      <c r="R48" s="3">
+        <v>100634</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
@@ -3129,8 +3199,8 @@
       <c r="Q49">
         <v>78665</v>
       </c>
-      <c r="R49" t="s">
-        <v>1</v>
+      <c r="R49" s="3">
+        <v>103157.73333333334</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
@@ -3185,8 +3255,8 @@
       <c r="Q50">
         <v>81979</v>
       </c>
-      <c r="R50" t="s">
-        <v>1</v>
+      <c r="R50" s="3">
+        <v>109813</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
@@ -3241,8 +3311,8 @@
       <c r="Q51">
         <v>93093</v>
       </c>
-      <c r="R51" t="s">
-        <v>1</v>
+      <c r="R51" s="3">
+        <v>118021.93333333333</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
@@ -3297,8 +3367,8 @@
       <c r="Q52">
         <v>74757</v>
       </c>
-      <c r="R52" t="s">
-        <v>1</v>
+      <c r="R52" s="3">
+        <v>116045.66666666667</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
@@ -3353,8 +3423,8 @@
       <c r="Q53">
         <v>60254</v>
       </c>
-      <c r="R53" t="s">
-        <v>1</v>
+      <c r="R53" s="3">
+        <v>110175.73333333334</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
@@ -3409,8 +3479,8 @@
       <c r="Q54">
         <v>82803</v>
       </c>
-      <c r="R54" t="s">
-        <v>1</v>
+      <c r="R54" s="3">
+        <v>112505.06666666667</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
@@ -3465,8 +3535,8 @@
       <c r="Q55">
         <v>85268</v>
       </c>
-      <c r="R55" t="s">
-        <v>1</v>
+      <c r="R55" s="3">
+        <v>120355</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
@@ -3521,8 +3591,8 @@
       <c r="Q56">
         <v>92897</v>
       </c>
-      <c r="R56" t="s">
-        <v>1</v>
+      <c r="R56" s="3">
+        <v>124521.2</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
@@ -3577,8 +3647,8 @@
       <c r="Q57">
         <v>88800</v>
       </c>
-      <c r="R57" t="s">
-        <v>1</v>
+      <c r="R57" s="3">
+        <v>131375.20000000001</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
@@ -3633,8 +3703,8 @@
       <c r="Q58">
         <v>92480</v>
       </c>
-      <c r="R58" t="s">
-        <v>1</v>
+      <c r="R58" s="3">
+        <v>130369.93333333333</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
@@ -3689,8 +3759,8 @@
       <c r="Q59">
         <v>62156</v>
       </c>
-      <c r="R59" t="s">
-        <v>1</v>
+      <c r="R59" s="3">
+        <v>128019.8</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
@@ -3745,8 +3815,8 @@
       <c r="Q60">
         <v>83347</v>
       </c>
-      <c r="R60" t="s">
-        <v>1</v>
+      <c r="R60" s="3">
+        <v>132064.46666666667</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
@@ -3801,8 +3871,8 @@
       <c r="Q61">
         <v>77344</v>
       </c>
-      <c r="R61" t="s">
-        <v>1</v>
+      <c r="R61" s="3">
+        <v>128172.4</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
@@ -3857,6 +3927,9 @@
       <c r="Q62">
         <v>70722</v>
       </c>
+      <c r="R62" s="3">
+        <v>140208.53333333333</v>
+      </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63">
@@ -3910,8 +3983,8 @@
       <c r="Q63">
         <v>69956</v>
       </c>
-      <c r="R63" t="s">
-        <v>1</v>
+      <c r="R63" s="3">
+        <v>130283.13333333333</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
@@ -3966,8 +4039,8 @@
       <c r="Q64">
         <v>73387</v>
       </c>
-      <c r="R64" t="s">
-        <v>1</v>
+      <c r="R64" s="3">
+        <v>131770</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
@@ -4022,8 +4095,8 @@
       <c r="Q65">
         <v>78353</v>
       </c>
-      <c r="R65" t="s">
-        <v>1</v>
+      <c r="R65" s="3">
+        <v>138326</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
@@ -4078,8 +4151,8 @@
       <c r="Q66">
         <v>81946</v>
       </c>
-      <c r="R66" t="s">
-        <v>1</v>
+      <c r="R66" s="3">
+        <v>145914.06666666668</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
@@ -4134,8 +4207,8 @@
       <c r="Q67">
         <v>109677</v>
       </c>
-      <c r="R67" t="s">
-        <v>1</v>
+      <c r="R67" s="3">
+        <v>143765.66666666666</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
@@ -4190,8 +4263,8 @@
       <c r="Q68">
         <v>78994</v>
       </c>
-      <c r="R68" t="s">
-        <v>1</v>
+      <c r="R68" s="3">
+        <v>147888.79999999999</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
@@ -4246,8 +4319,8 @@
       <c r="Q69">
         <v>79968</v>
       </c>
-      <c r="R69" t="s">
-        <v>1</v>
+      <c r="R69" s="3">
+        <v>137734</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
@@ -4302,8 +4375,8 @@
       <c r="Q70">
         <v>79916</v>
       </c>
-      <c r="R70" t="s">
-        <v>1</v>
+      <c r="R70" s="3">
+        <v>132208.33333333334</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
@@ -4358,8 +4431,8 @@
       <c r="Q71">
         <v>82156</v>
       </c>
-      <c r="R71" t="s">
-        <v>1</v>
+      <c r="R71" s="3">
+        <v>135821.6</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
@@ -4414,8 +4487,8 @@
       <c r="Q72">
         <v>82298</v>
       </c>
-      <c r="R72" t="s">
-        <v>1</v>
+      <c r="R72" s="3">
+        <v>143835.73333333334</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
@@ -4470,8 +4543,8 @@
       <c r="Q73">
         <v>85249</v>
       </c>
-      <c r="R73" t="s">
-        <v>1</v>
+      <c r="R73" s="3">
+        <v>147610.79999999999</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
@@ -4526,8 +4599,8 @@
       <c r="Q74">
         <v>89175</v>
       </c>
-      <c r="R74" t="s">
-        <v>1</v>
+      <c r="R74" s="3">
+        <v>156932.73333333334</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
@@ -4582,8 +4655,8 @@
       <c r="Q75">
         <v>99041</v>
       </c>
-      <c r="R75" t="s">
-        <v>1</v>
+      <c r="R75" s="3">
+        <v>154678.6</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
@@ -4638,8 +4711,8 @@
       <c r="Q76">
         <v>87950</v>
       </c>
-      <c r="R76" t="s">
-        <v>1</v>
+      <c r="R76" s="3">
+        <v>158354.06666666668</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
@@ -4694,8 +4767,8 @@
       <c r="Q77">
         <v>87123</v>
       </c>
-      <c r="R77" t="s">
-        <v>1</v>
+      <c r="R77" s="3">
+        <v>165411.53333333333</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
@@ -4750,8 +4823,8 @@
       <c r="Q78">
         <v>88803</v>
       </c>
-      <c r="R78" t="s">
-        <v>1</v>
+      <c r="R78" s="3">
+        <v>173707.13333333333</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
@@ -4806,8 +4879,8 @@
       <c r="Q79">
         <v>96301</v>
       </c>
-      <c r="R79" t="s">
-        <v>1</v>
+      <c r="R79" s="3">
+        <v>175848.4</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
@@ -4862,8 +4935,8 @@
       <c r="Q80">
         <v>109629</v>
       </c>
-      <c r="R80" t="s">
-        <v>1</v>
+      <c r="R80" s="3">
+        <v>175502.86666666667</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
@@ -4918,8 +4991,8 @@
       <c r="Q81">
         <v>127466</v>
       </c>
-      <c r="R81" t="s">
-        <v>1</v>
+      <c r="R81" s="3">
+        <v>176992</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
@@ -4974,8 +5047,8 @@
       <c r="Q82">
         <v>92166</v>
       </c>
-      <c r="R82" t="s">
-        <v>1</v>
+      <c r="R82" s="3">
+        <v>174611</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
@@ -5030,8 +5103,8 @@
       <c r="Q83">
         <v>101596</v>
       </c>
-      <c r="R83" t="s">
-        <v>1</v>
+      <c r="R83" s="3">
+        <v>177725.46666666667</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
@@ -5086,8 +5159,8 @@
       <c r="Q84">
         <v>86740</v>
       </c>
-      <c r="R84" t="s">
-        <v>1</v>
+      <c r="R84" s="3">
+        <v>183675.86666666667</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
@@ -5142,8 +5215,8 @@
       <c r="Q85">
         <v>97541</v>
       </c>
-      <c r="R85" t="s">
-        <v>1</v>
+      <c r="R85" s="3">
+        <v>175695.26666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>